<commit_message>
se me olvida que no hay que guardar y hacer commit
Hay que hacer guardar  + guardar  + guardar + commit
</commit_message>
<xml_diff>
--- a/SING_Practica_1/Datos.xlsx
+++ b/SING_Practica_1/Datos.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9045" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9045" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Transactional_read-only" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="11">
   <si>
     <t>Número de hilos</t>
   </si>
@@ -58,12 +58,15 @@
   <si>
     <t>NonTr_RO</t>
   </si>
+  <si>
+    <t>Comparativa dentro de la misma gráfica para cada uno de los parámetros estudiados</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -83,6 +86,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -215,7 +226,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -253,6 +264,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6796,7 +6810,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="es-ES"/>
-              <a:t>Coste </a:t>
+              <a:t>Eficiencia </a:t>
             </a:r>
             <a:r>
               <a:rPr lang="es-ES" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="0">
@@ -24094,7 +24108,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
@@ -25573,10 +25587,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E111"/>
+  <dimension ref="B1:H111"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="M78" sqref="M78"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25591,19 +25605,39 @@
     <col min="13" max="13" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E1" s="16"/>
+    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E2" s="16"/>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E3" s="16"/>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="E4" s="16"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="13" t="s">
         <v>3</v>
       </c>
@@ -25611,7 +25645,7 @@
       <c r="D5" s="13"/>
       <c r="E5" s="16"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>7</v>
       </c>
@@ -25623,10 +25657,7 @@
       </c>
       <c r="E6" s="16"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>1</v>
-      </c>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" s="14">
         <f>'Transactional_read-only'!F5</f>
         <v>99999.608189999999</v>
@@ -25641,10 +25672,7 @@
       </c>
       <c r="E7" s="16"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>2</v>
-      </c>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="14">
         <f>'Transactional_read-only'!F6</f>
         <v>99999.492748000004</v>
@@ -25659,10 +25687,7 @@
       </c>
       <c r="E8" s="16"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>3</v>
-      </c>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="14">
         <f>'Transactional_read-only'!F7</f>
         <v>100001.05788400001</v>
@@ -25677,10 +25702,7 @@
       </c>
       <c r="E9" s="16"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>4</v>
-      </c>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="14">
         <f>'Transactional_read-only'!F8</f>
         <v>100003.96122000001</v>
@@ -25695,10 +25717,7 @@
       </c>
       <c r="E10" s="16"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>5</v>
-      </c>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="14">
         <f>'Transactional_read-only'!F9</f>
         <v>100009.00303000001</v>
@@ -25713,10 +25732,7 @@
       </c>
       <c r="E11" s="16"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>6</v>
-      </c>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="14">
         <f>'Transactional_read-only'!F10</f>
         <v>100380.06355199999</v>
@@ -25731,10 +25747,7 @@
       </c>
       <c r="E12" s="16"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>7</v>
-      </c>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="14">
         <f>'Transactional_read-only'!F11</f>
         <v>100416.899401</v>
@@ -25749,10 +25762,7 @@
       </c>
       <c r="E13" s="16"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>8</v>
-      </c>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="14">
         <f>'Transactional_read-only'!F12</f>
         <v>100198.07979999999</v>
@@ -25767,10 +25777,7 @@
       </c>
       <c r="E14" s="16"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>9</v>
-      </c>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="14">
         <f>'Transactional_read-only'!F13</f>
         <v>100146.978516</v>
@@ -25785,10 +25792,7 @@
       </c>
       <c r="E15" s="16"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>10</v>
-      </c>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="14">
         <f>'Transactional_read-only'!F14</f>
         <v>100067.798964</v>
@@ -25803,10 +25807,7 @@
       </c>
       <c r="E16" s="16"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>11</v>
-      </c>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="14">
         <f>'Transactional_read-only'!F15</f>
         <v>100036.212424</v>
@@ -25821,10 +25822,7 @@
       </c>
       <c r="E17" s="16"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>12</v>
-      </c>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="14">
         <f>'Transactional_read-only'!F16</f>
         <v>100040.15980200001</v>
@@ -25839,10 +25837,7 @@
       </c>
       <c r="E18" s="16"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>13</v>
-      </c>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="14">
         <f>'Transactional_read-only'!F17</f>
         <v>100022.76066600002</v>
@@ -25857,10 +25852,7 @@
       </c>
       <c r="E19" s="16"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>14</v>
-      </c>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="14">
         <f>'Transactional_read-only'!F18</f>
         <v>100028.87972099999</v>
@@ -25875,10 +25867,7 @@
       </c>
       <c r="E20" s="16"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>15</v>
-      </c>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="14">
         <f>'Transactional_read-only'!F19</f>
         <v>100034.205246</v>
@@ -25893,10 +25882,7 @@
       </c>
       <c r="E21" s="16"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>16</v>
-      </c>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="14">
         <f>'Transactional_read-only'!F20</f>
         <v>100030.284508</v>
@@ -25911,10 +25897,7 @@
       </c>
       <c r="E22" s="16"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>17</v>
-      </c>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="14">
         <f>'Transactional_read-only'!F21</f>
         <v>100041.04955</v>
@@ -25929,10 +25912,7 @@
       </c>
       <c r="E23" s="16"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>18</v>
-      </c>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="14">
         <f>'Transactional_read-only'!F22</f>
         <v>100055.22600899999</v>
@@ -25947,10 +25927,7 @@
       </c>
       <c r="E24" s="16"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>19</v>
-      </c>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="14">
         <f>'Transactional_read-only'!F23</f>
         <v>100051.77084</v>
@@ -25965,10 +25942,7 @@
       </c>
       <c r="E25" s="16"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>20</v>
-      </c>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="14">
         <f>'Transactional_read-only'!F24</f>
         <v>100041.822139</v>
@@ -25983,10 +25957,7 @@
       </c>
       <c r="E26" s="16"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>21</v>
-      </c>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="14">
         <f>'Transactional_read-only'!F25</f>
         <v>100035.021987</v>
@@ -26001,10 +25972,7 @@
       </c>
       <c r="E27" s="16"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>22</v>
-      </c>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="14">
         <f>'Transactional_read-only'!F26</f>
         <v>100027.002867</v>
@@ -26019,10 +25987,7 @@
       </c>
       <c r="E28" s="16"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>23</v>
-      </c>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="14">
         <f>'Transactional_read-only'!F27</f>
         <v>100032.620142</v>
@@ -26037,7 +26002,7 @@
       </c>
       <c r="E29" s="16"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" s="13" t="s">
         <v>4</v>
       </c>
@@ -27058,13 +27023,15 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
+    <mergeCell ref="B1:H3"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="B32:D32"/>
     <mergeCell ref="B60:D60"/>
     <mergeCell ref="B87:D87"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
reparto de faena para la memoria.
</commit_message>
<xml_diff>
--- a/SING_Practica_1/Datos.xlsx
+++ b/SING_Practica_1/Datos.xlsx
@@ -17,6 +17,9 @@
     <sheet name="NoTransactional_read-only" sheetId="3" r:id="rId3"/>
     <sheet name="comparativa de las 3" sheetId="4" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'comparativa de las 3'!$B$88:$D$111</definedName>
+  </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -24468,8 +24471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:I27"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4:I4"/>
+    <sheetView topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25209,8 +25212,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:I27"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+    <sheetView topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25950,8 +25953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:I27"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="O54" sqref="O54"/>
+    <sheetView topLeftCell="A26" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26690,8 +26693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H111"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L58" sqref="L58"/>
+    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>